<commit_message>
updated Sprintplan. changed logout from pending to completed
</commit_message>
<xml_diff>
--- a/dokumente/Sprintberichte/Sprint 2/Sprint 2 - Übersicht.xlsx
+++ b/dokumente/Sprintberichte/Sprint 2/Sprint 2 - Übersicht.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8910" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8910"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2 Inhalt" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="108">
   <si>
     <t>Subtask</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Vom System abmelden</t>
-  </si>
-  <si>
-    <t>Teilweise</t>
   </si>
   <si>
     <t>Dauer / Aufwand</t>
@@ -673,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,13 +684,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
@@ -779,7 +776,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>0.5</v>
@@ -799,7 +796,7 @@
         <v>0.5</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -821,7 +818,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12">
         <v>0.5</v>
@@ -857,7 +854,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16">
         <v>0.4</v>
@@ -954,7 +951,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -963,7 +960,7 @@
         <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1113,7 +1110,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37">
         <v>1.5</v>
@@ -1127,7 +1124,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38">
         <v>0.5</v>
@@ -1173,7 +1170,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1182,85 +1179,85 @@
         <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
         <v>53</v>
-      </c>
-      <c r="D8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1285,23 +1282,23 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>0.2</v>
@@ -1309,7 +1306,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>0.3</v>
@@ -1317,7 +1314,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>0.2</v>
@@ -1325,12 +1322,12 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8">
         <v>0.5</v>
@@ -1338,7 +1335,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9">
         <v>0.2</v>
@@ -1346,7 +1343,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>0.2</v>
@@ -1354,7 +1351,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11">
         <v>0.1</v>
@@ -1362,12 +1359,12 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14">
         <v>0.2</v>
@@ -1375,7 +1372,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15">
         <v>0.3</v>
@@ -1383,12 +1380,12 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1396,7 +1393,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1404,7 +1401,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20">
         <v>0.5</v>
@@ -1412,7 +1409,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21">
         <v>0.1</v>
@@ -1420,12 +1417,12 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24">
         <v>0.2</v>
@@ -1433,7 +1430,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25">
         <v>0.8</v>
@@ -1441,7 +1438,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>0.5</v>
@@ -1449,12 +1446,12 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29">
         <v>0.1</v>
@@ -1462,7 +1459,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30">
         <v>0.5</v>
@@ -1470,12 +1467,12 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33">
         <v>0.5</v>
@@ -1483,7 +1480,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34">
         <v>0.8</v>
@@ -1491,7 +1488,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1499,7 +1496,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36">
         <v>0.1</v>
@@ -1507,12 +1504,12 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39">
         <v>0.2</v>
@@ -1520,7 +1517,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40">
         <v>0.6</v>
@@ -1528,7 +1525,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C41">
         <v>0.3</v>
@@ -1536,7 +1533,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42">
         <v>0.7</v>
@@ -1544,12 +1541,12 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C45">
         <v>0.2</v>
@@ -1557,7 +1554,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46">
         <v>0.5</v>
@@ -1565,7 +1562,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C47">
         <v>0.5</v>
@@ -1573,12 +1570,12 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50">
         <v>0.5</v>
@@ -1586,7 +1583,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C51">
         <v>0.5</v>
@@ -1599,7 +1596,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C54">
         <v>0.2</v>
@@ -1607,7 +1604,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C55">
         <v>0.3</v>
@@ -1615,12 +1612,12 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1628,27 +1625,27 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Sprintbericht for second Sprint. Fixed Burndowngraph (Jira to Excel). Fixed Sprintbacklog
</commit_message>
<xml_diff>
--- a/dokumente/Sprintberichte/Sprint 2/Sprint 2 - Übersicht.xlsx
+++ b/dokumente/Sprintberichte/Sprint 2/Sprint 2 - Übersicht.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2 Inhalt" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="108">
   <si>
     <t>Subtask</t>
   </si>
@@ -670,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1153,10 +1153,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,17 +1246,22 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>52</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>55</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E10" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1269,7 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>